<commit_message>
Production Entry and Item Master Changes(Dharmee)
</commit_message>
<xml_diff>
--- a/eTactWeb/wwwroot/Uploads/ImportSaleScheduleFormat (3).xlsx
+++ b/eTactWeb/wwwroot/Uploads/ImportSaleScheduleFormat (3).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Soumitra\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0627DD63-AD5F-40F4-9773-4857BF205F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30637A75-9318-4DC6-9ED4-8C76752C7CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -433,7 +433,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -481,7 +481,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="1">
-        <v>46481</v>
+        <v>45753</v>
       </c>
       <c r="E2">
         <v>12</v>

</xml_diff>